<commit_message>
se finalizan los 10 escenarios en kraken con ghost version 4
</commit_message>
<xml_diff>
--- a/kraken_tests_vnueva/InventarioEscenarios.xlsx
+++ b/kraken_tests_vnueva/InventarioEscenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\MISO\equipo3desarrollo\equipo3\kraken_tests_vnueva\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE71B8F-4501-4E63-9CCE-11690ECA7401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48AEB17-F52B-46B2-8A0C-16ECDD0E553C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-42210" yWindow="855" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
   <si>
     <t xml:space="preserve">Escenario </t>
   </si>
@@ -40,8 +40,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -69,8 +77,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,76 +361,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C9"/>
+  <dimension ref="B2:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5">
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6">
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7">
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8">
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9">
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C13" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>